<commit_message>
P1 - First submission
added practical significance boundary
</commit_message>
<xml_diff>
--- a/P7 - Design an A B Test/Calculations.xlsx
+++ b/P7 - Design an A B Test/Calculations.xlsx
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K115"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
P7 - 2nd submission
</commit_message>
<xml_diff>
--- a/P7 - Design an A B Test/Calculations.xlsx
+++ b/P7 - Design an A B Test/Calculations.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="111">
   <si>
     <t>Unique cookies to view page per day:</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>http://www.evanmiller.org/ab-testing/</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,6 +394,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -419,10 +430,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,8 +456,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -760,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K115"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,6 +947,9 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>110</v>
+      </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -974,14 +991,14 @@
         <v>0.01</v>
       </c>
       <c r="D24" s="9">
-        <f>5%/2</f>
-        <v>2.5000000000000001E-2</v>
+        <f>5%</f>
+        <v>0.05</v>
       </c>
       <c r="E24" s="8">
         <v>0.8</v>
       </c>
       <c r="F24">
-        <v>788450</v>
+        <v>651075</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
@@ -999,19 +1016,41 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="D25" s="9">
-        <f>5%/2</f>
-        <v>2.5000000000000001E-2</v>
+        <f>5%</f>
+        <v>0.05</v>
       </c>
       <c r="E25" s="8">
         <v>0.8</v>
       </c>
       <c r="F25">
-        <v>827150</v>
+        <v>683050</v>
       </c>
       <c r="G25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1">
+        <f>C15</f>
+        <v>0.53</v>
+      </c>
+      <c r="C26">
+        <v>0.01</v>
+      </c>
+      <c r="D26" s="9">
+        <f>5%</f>
+        <v>0.05</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F26">
+        <v>4655238</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -1029,7 +1068,7 @@
       </c>
       <c r="B30">
         <f>MAX(F24:F25)</f>
-        <v>827150</v>
+        <v>683050</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1055,7 +1094,7 @@
       </c>
       <c r="B35" s="11">
         <f>B30/(B33*B31)</f>
-        <v>20.678750000000001</v>
+        <v>17.076250000000002</v>
       </c>
       <c r="C35" t="s">
         <v>26</v>
@@ -1395,11 +1434,10 @@
       </c>
       <c r="B81" s="3">
         <f>_xlfn.NORM.S.INV(1-C81/2)</f>
-        <v>2.2414027276049464</v>
+        <v>1.9599639845400536</v>
       </c>
       <c r="C81" s="9">
-        <f>0.05/2</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D81" t="s">
         <v>93</v>
@@ -1411,7 +1449,7 @@
       </c>
       <c r="B82" s="3">
         <f>B81*B80</f>
-        <v>9.7986851326488187E-3</v>
+        <v>8.5683263071431003E-3</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,7 +1468,7 @@
       </c>
       <c r="B85" s="3">
         <f>B84-B82</f>
-        <v>-3.0353559713010382E-2</v>
+        <v>-2.9123200887504665E-2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1439,7 +1477,7 @@
       </c>
       <c r="B86" s="3">
         <f>B84+B82</f>
-        <v>-1.0756189447712746E-2</v>
+        <v>-1.1986548273218465E-2</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1495,11 +1533,10 @@
       </c>
       <c r="B94" s="3">
         <f>_xlfn.NORM.S.INV(1-C94/2)</f>
-        <v>2.2414027276049464</v>
+        <v>1.9599639845400536</v>
       </c>
       <c r="C94" s="9">
-        <f>0.05/2</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D94" t="s">
         <v>93</v>
@@ -1511,7 +1548,7 @@
       </c>
       <c r="B95" s="3">
         <f>B94*B93</f>
-        <v>7.6972762228462912E-3</v>
+        <v>6.730778003449565E-3</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -1529,7 +1566,7 @@
       </c>
       <c r="B98" s="3">
         <f>B97-B95</f>
-        <v>-1.2570998897390459E-2</v>
+        <v>-1.1604500677993733E-2</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -1538,7 +1575,7 @@
       </c>
       <c r="B99" s="3">
         <f>B97+B95</f>
-        <v>2.8235535483021237E-3</v>
+        <v>1.8570553289053975E-3</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -1562,7 +1599,7 @@
         <v>96</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -1605,7 +1642,7 @@
       <c r="B108">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="15" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1660,8 +1697,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A22" r:id="rId1"/>
+    <hyperlink ref="D108" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>